<commit_message>
added code base of POM - Part -5
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naveenkhunteta/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naveenkhunteta/Documents/workspace/FreeCRMTest/src/main/java/com/crm/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>